<commit_message>
requirements refactored + plug-in environment + apendix
</commit_message>
<xml_diff>
--- a/ThesisWork/requirements/value_matrix.xlsx
+++ b/ThesisWork/requirements/value_matrix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="24">
   <si>
     <t>Multiuser &amp; Access control</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Simplified access to social media</t>
+  </si>
+  <si>
+    <t>Data management</t>
+  </si>
+  <si>
+    <t>Scheduled execution</t>
   </si>
 </sst>
 </file>
@@ -189,10 +195,10 @@
                   <c:v>Plug-in environment</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scheduling</c:v>
+                  <c:v>Scheduled execution</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Universal datastore</c:v>
+                  <c:v>Data management</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Hadoop integration</c:v>
@@ -251,10 +257,10 @@
                   <c:v>Plug-in environment</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scheduling</c:v>
+                  <c:v>Scheduled execution</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Universal datastore</c:v>
+                  <c:v>Data management</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Hadoop integration</c:v>
@@ -313,10 +319,10 @@
                   <c:v>Plug-in environment</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scheduling</c:v>
+                  <c:v>Scheduled execution</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Universal datastore</c:v>
+                  <c:v>Data management</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Hadoop integration</c:v>
@@ -375,10 +381,10 @@
                   <c:v>Plug-in environment</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Scheduling</c:v>
+                  <c:v>Scheduled execution</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Universal datastore</c:v>
+                  <c:v>Data management</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Hadoop integration</c:v>
@@ -412,24 +418,24 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="65917696"/>
-        <c:axId val="65919232"/>
+        <c:axId val="61658240"/>
+        <c:axId val="61659776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="65917696"/>
+        <c:axId val="61658240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65919232"/>
+        <c:crossAx val="61659776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65919232"/>
+        <c:axId val="61659776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -437,7 +443,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65917696"/>
+        <c:crossAx val="61658240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -450,7 +456,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -516,24 +522,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="67114496"/>
-        <c:axId val="67116032"/>
+        <c:axId val="62207872"/>
+        <c:axId val="62209408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67114496"/>
+        <c:axId val="62207872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67116032"/>
+        <c:crossAx val="62209408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67116032"/>
+        <c:axId val="62209408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +547,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67114496"/>
+        <c:crossAx val="62207872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -550,7 +556,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -616,24 +622,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="68380928"/>
-        <c:axId val="68382720"/>
+        <c:axId val="81218176"/>
+        <c:axId val="81224064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68380928"/>
+        <c:axId val="81218176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68382720"/>
+        <c:crossAx val="81224064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68382720"/>
+        <c:axId val="81224064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +647,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68380928"/>
+        <c:crossAx val="81218176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -650,7 +656,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3040,7 +3046,7 @@
   <dimension ref="A2:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3170,7 +3176,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <f>'Geert-Jan'!H13/4</f>
@@ -3191,7 +3197,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <f>'Geert-Jan'!H14/4</f>

</xml_diff>